<commit_message>
Lambdas & Notes in excel
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIRISHAA\IdeaProjects\javaFundamentals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalya\IdeaProjects\javaFundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{B0828C96-52ED-4343-B750-5867C9FE0294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="838" activeTab="12"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Access Specifiers" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,12 @@
     <sheet name="Nested Classes-Oracle" sheetId="10" r:id="rId10"/>
     <sheet name="Generics" sheetId="12" r:id="rId11"/>
     <sheet name="LambdaExpressions" sheetId="11" r:id="rId12"/>
-    <sheet name="Streaming&amp;API" sheetId="13" r:id="rId13"/>
+    <sheet name="Streaming API" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="kalyan chavali - Personal View" guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="11"/>
     <customWorkbookView name="SIRISHA AYYAGARI - Personal View" guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" autoUpdate="1" mergeInterval="15" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="838" activeSheetId="13"/>
-    <customWorkbookView name="kalyan chavali - Personal View" guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="11"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,12 +47,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>SIRISHA AYYAGARI</author>
   </authors>
   <commentList>
-    <comment ref="E37" authorId="0" guid="{78D41D66-65EF-455C-B883-EC918809DAC6}" shapeId="0">
+    <comment ref="E37" authorId="0" guid="{78D41D66-65EF-455C-B883-EC918809DAC6}" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D46" authorId="0" guid="{D695C8B9-1E70-46E7-8787-BAA0EB7801B1}" shapeId="0">
+    <comment ref="D46" authorId="0" guid="{D695C8B9-1E70-46E7-8787-BAA0EB7801B1}" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -2764,9 +2765,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -3065,7 +3066,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -7301,7 +7302,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
@@ -7567,11 +7568,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7628,12 +7629,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+      <selection activeCell="C12" sqref="C12"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="C11" sqref="C11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
-      <selection activeCell="C12" sqref="C12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -7642,7 +7643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="C2:J49"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -7766,11 +7767,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A13">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A13">
       <selection activeCell="J28" sqref="J28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A13">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A13">
       <selection activeCell="J28" sqref="J28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -7781,11 +7782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="C4:K79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8120,26 +8121,27 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
-      <selection activeCell="D8" sqref="D8"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A48">
       <selection activeCell="D53" sqref="D53"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+      <selection activeCell="D8" sqref="D8"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="D6:N58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8460,13 +8462,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A7">
-      <selection activeCell="H29" sqref="H29"/>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A30">
+      <selection activeCell="E49" sqref="E49"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A30">
-      <selection activeCell="E49" sqref="E49"/>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A7">
+      <selection activeCell="H29" sqref="H29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>
@@ -8477,11 +8479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="D5:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8731,23 +8733,22 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+      <selection activeCell="B16" sqref="B16"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A35">
       <selection activeCell="E42" sqref="E42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
-      <selection activeCell="B16" sqref="B16"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8918,19 +8919,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="B5" sqref="B5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="B5" sqref="B5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="F15" r:id="rId3" display="https://beginnersbook.com/2013/12/java-constructor-in-interface/"/>
+    <hyperlink ref="F15" r:id="rId3" display="https://beginnersbook.com/2013/12/java-constructor-in-interface/" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -8938,7 +8939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8954,11 +8955,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -8968,7 +8969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B4:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9120,11 +9121,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="H16" sqref="H16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="H16" sqref="H16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -9135,7 +9136,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C5:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9187,12 +9188,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -9204,7 +9205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9245,11 +9246,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="C19" sqref="C19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="C19" sqref="C19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -9259,7 +9260,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B4:D43"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -9449,19 +9450,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A19">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A19">
       <selection activeCell="F25" sqref="F25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A19">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A19">
       <selection activeCell="F25" sqref="F25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="C9" r:id="rId3" display="http://www.oracle.com/technetwork/java/codeconventions-135099.html"/>
+    <hyperlink ref="C9" r:id="rId3" display="http://www.oracle.com/technetwork/java/codeconventions-135099.html" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -9469,7 +9470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B4:O42"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -9681,12 +9682,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A31">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A31">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A31">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A31">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -9698,7 +9699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="C5:F122"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -10296,12 +10297,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" showPageBreaks="1" topLeftCell="B1">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="B1">
       <selection activeCell="D119" sqref="D119"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="B1">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" showPageBreaks="1" topLeftCell="B1">
       <selection activeCell="D119" sqref="D119"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
FIle IO notes added
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalya\IdeaProjects\JavaFundamental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{AE0C2EEA-610D-432E-AE7A-478D0AE445B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{C6359D5A-1998-4762-B2C2-2563E0720847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="17" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="17" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Access Specifiers" sheetId="1" r:id="rId1"/>
@@ -37,8 +37,8 @@
   </sheets>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="SIRISHA AYYAGARI - Personal View" guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" autoUpdate="1" mergeInterval="15" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="838" activeSheetId="18"/>
     <customWorkbookView name="kalyan chavali - Personal View" guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="20"/>
-    <customWorkbookView name="SIRISHA AYYAGARI - Personal View" guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" autoUpdate="1" mergeInterval="15" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="838" activeSheetId="18"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="864">
   <si>
     <t>It resembles a method but it is not a method.</t>
   </si>
@@ -4730,6 +4730,87 @@
   </si>
   <si>
     <t>Constructors in File Class</t>
+  </si>
+  <si>
+    <t>There are 3 constructors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File f = new File(String name); </t>
+  </si>
+  <si>
+    <t>it may be file name or directory name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When we want to create a file (abc.txt) in current working directory or creating a directory(siri123) in current working directory then we have to use the above constructor </t>
+  </si>
+  <si>
+    <t>To create a file/ directory in current working directory</t>
+  </si>
+  <si>
+    <t>To represent resources in CWD</t>
+  </si>
+  <si>
+    <t>File f = new File("siri123","abc.txt")</t>
+  </si>
+  <si>
+    <t>If you want to create a file or directory present in some other directory other than CWD, then we should use this constructor</t>
+  </si>
+  <si>
+    <t>File f= new File(String subdirname, String name)</t>
+  </si>
+  <si>
+    <t>File f = new File(File subdir, String name)</t>
+  </si>
+  <si>
+    <t>File f= new File(f1,"abc.txt")</t>
+  </si>
+  <si>
+    <t>If you want to create a file in a directory, where there exists already a file in the same directory, then the file name can be given instead of specifying the directory name</t>
+  </si>
+  <si>
+    <t>To represent resources in some other directory</t>
+  </si>
+  <si>
+    <t>Write a code to create a file named demo.txt in CWD</t>
+  </si>
+  <si>
+    <t>File f = new File ("demo.txt);</t>
+  </si>
+  <si>
+    <t>f.createNewFile();</t>
+  </si>
+  <si>
+    <t>Ex:1</t>
+  </si>
+  <si>
+    <t>Ex:2</t>
+  </si>
+  <si>
+    <t>Create a directory named "durga123" in CWD and create a file named "abc.txt"in the same directory.</t>
+  </si>
+  <si>
+    <t>File f = new File ("durga123");</t>
+  </si>
+  <si>
+    <t>f.mkdir();</t>
+  </si>
+  <si>
+    <t>File f1 = new File ("durga123","abc.txt");</t>
+  </si>
+  <si>
+    <t>File f1 = new File (f,"abc.txt");</t>
+  </si>
+  <si>
+    <t>f1.createNewFile();</t>
+  </si>
+  <si>
+    <t>Ex:3</t>
+  </si>
+  <si>
+    <t>Create a file named abc.txt in folder E:/xyz</t>
+  </si>
+  <si>
+    <t>File f = new File ("E://xyz",abc.txt);</t>
   </si>
 </sst>
 </file>
@@ -5739,7 +5820,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{160D7978-7907-4E89-8A2D-A01D7BE7A139}" diskRevisions="1" revisionId="1041" version="44">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3CEB751A-A69A-47A6-A3DC-4FD2FA079779}" diskRevisions="1" revisionId="1089" version="49">
   <header guid="{4E5BEA1C-670B-461C-B13D-48FC784813E1}" dateTime="2020-01-28T10:58:52" maxSheetId="18" userName="SIRISHA AYYAGARI" r:id="rId81" minRId="442" maxRId="454">
     <sheetIdMap count="17">
       <sheetId val="1"/>
@@ -6484,6 +6565,131 @@
       <sheetId val="21"/>
     </sheetIdMap>
   </header>
+  <header guid="{FFDBED6B-D6DD-4299-BC69-D584A939151F}" dateTime="2020-02-24T21:33:41" maxSheetId="22" userName="kalyan chavali" r:id="rId115" minRId="1042" maxRId="1063">
+    <sheetIdMap count="21">
+      <sheetId val="1"/>
+      <sheetId val="18"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+      <sheetId val="12"/>
+      <sheetId val="11"/>
+      <sheetId val="13"/>
+      <sheetId val="14"/>
+      <sheetId val="15"/>
+      <sheetId val="16"/>
+      <sheetId val="17"/>
+      <sheetId val="19"/>
+      <sheetId val="20"/>
+      <sheetId val="21"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{95F87900-9306-4D5A-B184-1D1D15CF8032}" dateTime="2020-02-24T21:40:14" maxSheetId="22" userName="kalyan chavali" r:id="rId116" minRId="1064" maxRId="1066">
+    <sheetIdMap count="21">
+      <sheetId val="1"/>
+      <sheetId val="18"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+      <sheetId val="12"/>
+      <sheetId val="11"/>
+      <sheetId val="13"/>
+      <sheetId val="14"/>
+      <sheetId val="15"/>
+      <sheetId val="16"/>
+      <sheetId val="17"/>
+      <sheetId val="19"/>
+      <sheetId val="20"/>
+      <sheetId val="21"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{21555528-F7C1-4032-8B8A-AC18AB73E5EA}" dateTime="2020-02-24T21:45:44" maxSheetId="22" userName="kalyan chavali" r:id="rId117" minRId="1067" maxRId="1080">
+    <sheetIdMap count="21">
+      <sheetId val="1"/>
+      <sheetId val="18"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+      <sheetId val="12"/>
+      <sheetId val="11"/>
+      <sheetId val="13"/>
+      <sheetId val="14"/>
+      <sheetId val="15"/>
+      <sheetId val="16"/>
+      <sheetId val="17"/>
+      <sheetId val="19"/>
+      <sheetId val="20"/>
+      <sheetId val="21"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{75441A11-65F5-4026-9D25-D96F1A6BB298}" dateTime="2020-02-24T21:52:10" maxSheetId="22" userName="kalyan chavali" r:id="rId118" minRId="1081" maxRId="1089">
+    <sheetIdMap count="21">
+      <sheetId val="1"/>
+      <sheetId val="18"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+      <sheetId val="12"/>
+      <sheetId val="11"/>
+      <sheetId val="13"/>
+      <sheetId val="14"/>
+      <sheetId val="15"/>
+      <sheetId val="16"/>
+      <sheetId val="17"/>
+      <sheetId val="19"/>
+      <sheetId val="20"/>
+      <sheetId val="21"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3CEB751A-A69A-47A6-A3DC-4FD2FA079779}" dateTime="2020-02-24T22:29:31" maxSheetId="22" userName="kalyan chavali" r:id="rId119">
+    <sheetIdMap count="21">
+      <sheetId val="1"/>
+      <sheetId val="18"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+      <sheetId val="12"/>
+      <sheetId val="11"/>
+      <sheetId val="13"/>
+      <sheetId val="14"/>
+      <sheetId val="15"/>
+      <sheetId val="16"/>
+      <sheetId val="17"/>
+      <sheetId val="19"/>
+      <sheetId val="20"/>
+      <sheetId val="21"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -10625,6 +10831,315 @@
   </rcc>
   <rcv guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" action="delete"/>
   <rcv guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1042" sId="21" eol="1" ref="A34:XFD34" action="insertRow"/>
+  <rcc rId="1043" sId="21">
+    <nc r="B34" t="inlineStr">
+      <is>
+        <t>There are 3 constructors</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1044" sId="21" eol="1" ref="A35:XFD35" action="insertRow"/>
+  <rcc rId="1045" sId="21">
+    <nc r="B35" t="inlineStr">
+      <is>
+        <t xml:space="preserve">File f = new File(String name); </t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1046" sId="21">
+    <nc r="E35" t="inlineStr">
+      <is>
+        <t>it may be file name or directory name</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1047" sId="21" eol="1" ref="A36:XFD36" action="insertRow"/>
+  <rcc rId="1048" sId="21">
+    <nc r="B36" t="inlineStr">
+      <is>
+        <t xml:space="preserve">When we want to create a file (abc.txt) in current working directory or creating a directory(siri123) in current working directory then we have to use the above constructor </t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1049" sId="21" eol="1" ref="A37:XFD37" action="insertRow"/>
+  <rcc rId="1050" sId="21">
+    <nc r="B37" t="inlineStr">
+      <is>
+        <t>To create a file/ directory in current working directory</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1051" sId="21" eol="1" ref="A38:XFD38" action="insertRow"/>
+  <rcc rId="1052" sId="21">
+    <nc r="B38" t="inlineStr">
+      <is>
+        <t>To represent resources in CWD</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="21" sqref="B35" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="1053" sId="21">
+    <nc r="A35">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcc rId="1054" sId="21">
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>File f = new File("siri123","abc.txt")</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1055" sId="21" eol="1" ref="A41:XFD41" action="insertRow"/>
+  <rcc rId="1056" sId="21">
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>If you want to create a file or directory present in some other directory other than CWD, then we should use this constructor</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1057" sId="21" ref="A40:XFD40" action="insertRow"/>
+  <rcc rId="1058" sId="21">
+    <nc r="A40">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="1059" sId="21">
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>File f= new File(String subdirname, String name)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1060" sId="21">
+    <nc r="A44">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="21" sqref="B40" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="1061" sId="21">
+    <nc r="B44" t="inlineStr">
+      <is>
+        <t>File f = new File(File subdir, String name)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1062" sId="21">
+    <nc r="B45" t="inlineStr">
+      <is>
+        <t>File f= new File(f1,"abc.txt")</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1063" sId="21">
+    <nc r="B46" t="inlineStr">
+      <is>
+        <t>If you want to create a file in a directory, where there exists already a file in the same directory, then the file name can be given instead of specifying the directory name</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="21" sqref="B44" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1064" sId="21" ref="A43:XFD43" action="insertRow"/>
+  <rcc rId="1065" sId="21">
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>To represent resources in some other directory</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1066" sId="21">
+    <nc r="B48" t="inlineStr">
+      <is>
+        <t>To represent resources in some other directory</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1067" sId="21">
+    <nc r="B51" t="inlineStr">
+      <is>
+        <t>Write a code to create a file named demo.txt in CWD</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1068" sId="21" eol="1" ref="A52:XFD52" action="insertRow"/>
+  <rcc rId="1069" sId="21">
+    <nc r="B52" t="inlineStr">
+      <is>
+        <t>File f = new File ("demo.txt);</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1070" sId="21" eol="1" ref="A53:XFD53" action="insertRow"/>
+  <rcc rId="1071" sId="21">
+    <nc r="B53" t="inlineStr">
+      <is>
+        <t>f.createNewFile();</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1072" sId="21" ref="A50:XFD50" action="insertRow"/>
+  <rcc rId="1073" sId="21">
+    <nc r="B51" t="inlineStr">
+      <is>
+        <t>Ex:1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1074" sId="21">
+    <nc r="B56" t="inlineStr">
+      <is>
+        <t>Ex:2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1075" sId="21" eol="1" ref="A57:XFD57" action="insertRow"/>
+  <rcc rId="1076" sId="21">
+    <nc r="B57" t="inlineStr">
+      <is>
+        <t>Create a directory named "durga123" in CWD and create a file named "abc.txt"in the same directory.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1077" sId="21">
+    <nc r="B58" t="inlineStr">
+      <is>
+        <t>File f = new File ("durga123");</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1078" sId="21">
+    <nc r="B59" t="inlineStr">
+      <is>
+        <t>f.mkdir();</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1079" sId="21">
+    <nc r="B61" t="inlineStr">
+      <is>
+        <t>f.createNewFile();</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1080" sId="21">
+    <nc r="B60" t="inlineStr">
+      <is>
+        <t>File f = new File ("abc.txt");</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1081" sId="21">
+    <oc r="B60" t="inlineStr">
+      <is>
+        <t>File f = new File ("abc.txt");</t>
+      </is>
+    </oc>
+    <nc r="B60" t="inlineStr">
+      <is>
+        <t>File f1 = new File ("durga123","abc.txt");</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="1082" sheetId="21" source="B61" destination="B62" sourceSheetId="21"/>
+  <rcc rId="1083" sId="21">
+    <nc r="B61" t="inlineStr">
+      <is>
+        <t>File f1 = new File (f,"abc.txt");</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1084" sId="21">
+    <oc r="B62" t="inlineStr">
+      <is>
+        <t>f.createNewFile();</t>
+      </is>
+    </oc>
+    <nc r="B62" t="inlineStr">
+      <is>
+        <t>f1.createNewFile();</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1085" sId="21">
+    <nc r="B64" t="inlineStr">
+      <is>
+        <t>Ex:3</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="1086" sId="21" eol="1" ref="A65:XFD65" action="insertRow"/>
+  <rcc rId="1087" sId="21">
+    <nc r="B65" t="inlineStr">
+      <is>
+        <t>Create a file named abc.txt in folder E:/xyz</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1088" sId="21">
+    <nc r="B66" t="inlineStr">
+      <is>
+        <t>File f = new File ("E://xyz",abc.txt);</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1089" sId="21">
+    <nc r="B67" t="inlineStr">
+      <is>
+        <t>f.createNewFile();</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="21" sqref="B51 B56 B64" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
 </revisions>
 </file>
 
@@ -14637,12 +15152,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+      <selection activeCell="C11" sqref="C11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="C12" sqref="C12"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
-      <selection activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -15269,12 +15784,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="B1">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" showPageBreaks="1" topLeftCell="B4">
       <selection activeCell="D119" sqref="D119"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" showPageBreaks="1" topLeftCell="B4">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="B1">
       <selection activeCell="D119" sqref="D119"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -15432,11 +15947,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A13">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A13">
       <selection activeCell="J28" sqref="J28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A13">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A13">
       <selection activeCell="J28" sqref="J28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -15806,14 +16321,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A7">
+      <selection activeCell="D8" sqref="D8"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A48">
       <selection activeCell="D53" sqref="D53"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-    </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A7">
-      <selection activeCell="D8" sqref="D8"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16167,13 +16682,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A30">
-      <selection activeCell="E49" sqref="E49"/>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A19">
+      <selection activeCell="H29" sqref="H29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A19">
-      <selection activeCell="H29" sqref="H29"/>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A30">
+      <selection activeCell="E49" sqref="E49"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>
@@ -16458,14 +16973,14 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
-      <selection activeCell="B16" sqref="B16"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A35">
       <selection activeCell="R73" sqref="R73"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+      <selection activeCell="B16" sqref="B16"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17057,13 +17572,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" scale="80" topLeftCell="A43">
-      <selection activeCell="G54" sqref="G54"/>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A46">
+      <selection activeCell="F64" sqref="F64"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A46">
-      <selection activeCell="F64" sqref="F64"/>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" scale="80" topLeftCell="A43">
+      <selection activeCell="G54" sqref="G54"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>
@@ -17987,13 +18502,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A61">
-      <selection activeCell="B10" sqref="B10"/>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A61">
+      <selection activeCell="C19" sqref="C19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A61">
-      <selection activeCell="C19" sqref="C19"/>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A61">
+      <selection activeCell="B10" sqref="B10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>
@@ -18060,12 +18575,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+      <selection activeCell="E11" sqref="E11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="B10" sqref="B10"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
-      <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -18275,13 +18790,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A37">
-      <selection activeCell="E42" sqref="E42"/>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+      <selection activeCell="E22" sqref="E22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
-      <selection activeCell="E22" sqref="E22"/>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A37">
+      <selection activeCell="E42" sqref="E42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -18296,7 +18811,7 @@
   <dimension ref="D2:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18471,11 +18986,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="B10" sqref="B10"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -18487,8 +19002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDB8E36-13BC-4FC7-BC13-7ABFB4668CB2}">
   <dimension ref="A4:M113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19327,10 +19842,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42CB821-9A2F-43EC-9633-352DC1419B24}">
-  <dimension ref="B2:J33"/>
+  <dimension ref="A2:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19474,9 +19989,161 @@
         <v>835</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="79" t="s">
         <v>836</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="79" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="79">
+        <v>1</v>
+      </c>
+      <c r="B35" s="80" t="s">
+        <v>838</v>
+      </c>
+      <c r="E35" s="79" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="79" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="79" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="79" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="79">
+        <v>2</v>
+      </c>
+      <c r="B40" s="80" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="79" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="79" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="79" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="79">
+        <v>3</v>
+      </c>
+      <c r="B45" s="80" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="79" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="79" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="79" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="80" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="79" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="79" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="79" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="80" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="79" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="79" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="79" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="79" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="79" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="79" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="80" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="79" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="79" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="79" t="s">
+        <v>852</v>
       </c>
     </row>
   </sheetData>
@@ -19487,6 +20154,7 @@
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19682,12 +20350,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="B5" sqref="B5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="B5" sqref="B5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -19738,11 +20406,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -19924,11 +20592,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="H16" sqref="H16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="H16" sqref="H16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -20011,13 +20679,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+      <selection activeCell="D12" sqref="D12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
-      <selection activeCell="D12" sqref="D12"/>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>
@@ -20089,11 +20757,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
       <selection activeCell="C19" sqref="C19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}">
       <selection activeCell="C19" sqref="C19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -20313,12 +20981,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A19">
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A13">
       <selection activeCell="F25" sqref="F25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A13">
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A19">
       <selection activeCell="F25" sqref="F25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -20597,13 +21265,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A31">
-      <selection activeCell="C41" sqref="C41"/>
+    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A29">
+      <selection activeCell="C43" sqref="C43"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ADB1B302-3041-4CA3-9A15-0696EC45EC4B}" topLeftCell="A29">
-      <selection activeCell="C43" sqref="C43"/>
+    <customSheetView guid="{B388384C-8642-4245-BBEF-8F07AC3839C5}" topLeftCell="A31">
+      <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>

</xml_diff>